<commit_message>
:bug: Fixing bug sending image
sending images
</commit_message>
<xml_diff>
--- a/chats/5219982424394@c.us.xlsx
+++ b/chats/5219982424394@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Fecha</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Mensajes</t>
   </si>
   <si>
-    <t>11-10-2021 10:57</t>
+    <t>13-10-2021 01:15</t>
   </si>
   <si>
     <t xml:space="preserve">👋 Hola Gracias por contactarnos!
@@ -28,93 +28,18 @@
  🔵  Si deseas obtener información sobre Verificaciones Vehiculares escribe la palabra *"VERIFICACION"* 
  🔵  Si deseas obtener información la licencia federal escribe la palabra *"LICENCIA"* 
  🔵  Si deseas obtener información sobre ALTA/BAJA de Placas ante la SCT escribe la palabra  *"PLACAS"* 
- ✅ Información general sobre los cursos de capacitación vehicular ⮕ https://bit.ly/3od1Bl6  Visita nuestro sitio web para más información ⮕ https://bit.ly/3pg1Q02 
+  Visita nuestro sitio web para más información ⮕ https://mochcun.com 
 </t>
   </si>
   <si>
-    <t>11-10-2021 10:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">👋 Has elefido la opcion de pendejeta 
- Recuerda subscribirte a mi canal de YT ------ ------ Veo que es la primera vez que nos escribes ¿Quieres que te envie un MEME? Responde Quieromeme</t>
-  </si>
-  <si>
-    <t>11-10-2021 11:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">👋 Has elegido la opcion de placas 
-</t>
-  </si>
-  <si>
-    <t>12-10-2021 12:11</t>
-  </si>
-  <si>
-    <t>12-10-2021 12:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">👋 Has elegido la opcion de direccion 
-</t>
-  </si>
-  <si>
-    <t>12-10-2021 12:27</t>
-  </si>
-  <si>
-    <t>12-10-2021 03:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🚘 ALTA
- 👋 Has elegido la opcion de placas 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🚘 Estamos ubicados en Av. Kinik Lote 1-11, 1-12, 1-13 Mza. 1 Reg. 97 Zona Industrial. Entre la Av. Andres Q.roo y la Av. Chichen, casi llegando a la Chichen. Rejas Rojas. Frente a la Cerveceria Moctezuna | Superior. 
+    <t xml:space="preserve">🚘 Estamos ubicados en Av. Kinik Lote 1-11, 1-12, 1-13 Mza. 1 Reg. 97 Zona Industrial. Entre la Av. Andres Q.roo y la Av. Chichen sobre la kinik casi llegando a la Chichen. Rejas Rojas. Frente a la Cerveceria Moctezuna. 
  https://g.page/Mochcun?share 
 </t>
   </si>
   <si>
-    <t>12-10-2021 03:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🚘 Haz elegido la opción de verificacion, ¿En qué estas interesado? 
- ✔️ Para precio de Verificaciones escribe *COSTOS* 
- ✔️ Para información de Verificacion de Emisiones Contaminantes escribe *EMISIONES*
- ✔️ Para información de Verificacion de Fisico Mécanica escribe *FISICO*
- ✔️ Tienes duda si tu vehiculo cuenta con prorroga? escribe *PRORROGA*
-</t>
-  </si>
-  <si>
-    <t>12-10-2021 03:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">👋 Hola Gracias por contactarnos!
- 🚗 Te estás comunicando a la asistente del verificentro *MOCHCUN* 🚗  
- 🔵  Si deseas obtener la dirección de nuestro centro de verificación vehicular escribe la palabra *"DIRECCION"* 
- 🔵  Si deseas obtener información sobre Verificaciones Vehiculares escribe la palabra *"VERIFICACION"* 
- 🔵  Si deseas obtener información la licencia federal escribe la palabra *"LICENCIA"* 
-  Visita nuestro sitio web para más información ⮕ https://mochcun.com 
-</t>
-  </si>
-  <si>
-    <t>12-10-2021 03:33</t>
-  </si>
-  <si>
-    <t>12-10-2021 03:44</t>
-  </si>
-  <si>
-    <t>12-10-2021 04:36</t>
-  </si>
-  <si>
-    <t>12-10-2021 04:37</t>
-  </si>
-  <si>
-    <t>12-10-2021 04:39</t>
-  </si>
-  <si>
-    <t>12-10-2021 10:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🚘 Estamos ubicados en Av. Kinik Lote 1-11, 1-12, 1-13 Mza. 1 Reg. 97 Zona Industrial. Entre la Av. Andres Q.roo y la Av. Chichen sobre la kinik casi llegando a la Chichen. Rejas Rojas. Frente a la Cerveceria Moctezuna. 
- https://g.page/Mochcun?share 
+    <t xml:space="preserve">👋 Has elegido la opcion de placas, ¿En qué estas interesado?  
+ 🚘 ALTA DE PLACAS ANTE LA SCT 
+ 🚘 BAJA DE PLACAS ANTE LA SCT
 </t>
   </si>
   <si>
@@ -124,6 +49,15 @@
  ✔️ Para requisitos de la licencia escribe *Requisitos licencia*
  ✔️ Para costos de gestoria de la licencia escribe *costos licencia*
 </t>
+  </si>
+  <si>
+    <t>13-10-2021 01:21</t>
+  </si>
+  <si>
+    <t>13-10-2021 01:28</t>
+  </si>
+  <si>
+    <t>13-10-2021 08:51</t>
   </si>
 </sst>
 </file>
@@ -500,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,42 +455,42 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,119 +498,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>